<commit_message>
added excel manipulation, removed list comprehension in walrused-send_cmd_to_ssh.py
</commit_message>
<xml_diff>
--- a/excel/Test.xlsx
+++ b/excel/Test.xlsx
@@ -430,13 +430,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="17.21875" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
@@ -553,7 +553,36 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B13">
+        <f>SUM(A2:A11)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="00E0FFFF"/>
+        <color rgb="00008080"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="00E0FFFF"/>
+        <color rgb="00008080"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>